<commit_message>
Remove unused template import and add today's date to the worksheet
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Production follow up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8876AC-2768-43A0-83A2-A947B620EBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6FB6D6-5CB7-441A-A5FC-13385AE2D0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,7 +611,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
       </c>
       <c r="B2" s="5">
         <f ca="1">TODAY() - 1</f>
-        <v>45806</v>
+        <v>45809</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -726,12 +726,12 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10">
-        <v>4135752</v>
+        <v>1827707</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10">
         <f>C4-D4</f>
-        <v>4135752</v>
+        <v>1827707</v>
       </c>
       <c r="F4" s="10">
         <f>C4*W4/V4</f>
@@ -743,11 +743,11 @@
       </c>
       <c r="H4" s="10">
         <f>(E4+B4)/(X4+1)</f>
-        <v>147705.42857142858</v>
+        <v>96195.105263157893</v>
       </c>
       <c r="I4" s="10">
         <f>H4*N4</f>
-        <v>1141762.962857143</v>
+        <v>662784.27526315791</v>
       </c>
       <c r="J4" s="10">
         <f>B4*O4</f>
@@ -760,18 +760,18 @@
       </c>
       <c r="M4" s="10">
         <f>H4/P4</f>
-        <v>14995.474981870922</v>
+        <v>9835.9003336562273</v>
       </c>
       <c r="N4" s="9">
-        <v>7.73</v>
+        <v>6.89</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9">
-        <v>9.85</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="12">
-        <v>0.68</v>
+        <v>0.69</v>
       </c>
       <c r="S4" s="12"/>
       <c r="T4" s="10">
@@ -783,12 +783,12 @@
         <v>0</v>
       </c>
       <c r="V4" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9">
         <f>V4-W4</f>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -797,12 +797,12 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10">
-        <v>253849</v>
+        <v>221717</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10">
         <f t="shared" ref="E5:E13" si="0">C5-D5</f>
-        <v>253849</v>
+        <v>221717</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" ref="F5:F13" si="1">C5*W5/V5</f>
@@ -814,11 +814,11 @@
       </c>
       <c r="H5" s="10">
         <f t="shared" ref="H5:H13" si="3">(E5+B5)/(X5+1)</f>
-        <v>9066.0357142857138</v>
+        <v>11669.315789473685</v>
       </c>
       <c r="I5" s="10">
         <f t="shared" ref="I5:I13" si="4">H5*N5</f>
-        <v>59745.175357142849</v>
+        <v>73983.462105263156</v>
       </c>
       <c r="J5" s="10">
         <f t="shared" ref="J5:J13" si="5">B5*O5</f>
@@ -831,18 +831,18 @@
       </c>
       <c r="M5" s="18">
         <f t="shared" ref="M5:M13" si="7">H5/P5</f>
-        <v>920.40971718636695</v>
+        <v>1193.1815735658165</v>
       </c>
       <c r="N5" s="9">
-        <v>6.59</v>
+        <v>6.34</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9">
-        <v>9.85</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="12">
-        <v>0.63</v>
+        <v>0.67</v>
       </c>
       <c r="S5" s="12"/>
       <c r="T5" s="10">
@@ -854,12 +854,12 @@
         <v>0</v>
       </c>
       <c r="V5" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W5" s="9"/>
       <c r="X5" s="9">
         <f t="shared" ref="X5:X13" si="10">V5-W5</f>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -868,12 +868,12 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10">
-        <v>1950813</v>
+        <v>2096181</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10">
         <f t="shared" si="0"/>
-        <v>1950813</v>
+        <v>2096181</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="1"/>
@@ -885,11 +885,11 @@
       </c>
       <c r="H6" s="10">
         <f t="shared" si="3"/>
-        <v>69671.892857142855</v>
+        <v>110325.31578947368</v>
       </c>
       <c r="I6" s="10">
         <f t="shared" si="4"/>
-        <v>418728.07607142854</v>
+        <v>692842.98315789469</v>
       </c>
       <c r="J6" s="10">
         <f t="shared" si="5"/>
@@ -902,18 +902,18 @@
       </c>
       <c r="M6" s="10">
         <f t="shared" si="7"/>
-        <v>7073.2886149383612</v>
+        <v>10339.767178020027</v>
       </c>
       <c r="N6" s="9">
-        <v>6.01</v>
+        <v>6.28</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="9">
-        <v>9.85</v>
+        <v>10.67</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="12">
-        <v>0.72799999999999998</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="S6" s="12"/>
       <c r="T6" s="10">
@@ -925,12 +925,12 @@
         <v>0</v>
       </c>
       <c r="V6" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W6" s="9"/>
       <c r="X6" s="9">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -939,12 +939,12 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10">
-        <v>2338298</v>
+        <v>1388642</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10">
         <f t="shared" si="0"/>
-        <v>2338298</v>
+        <v>1388642</v>
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
@@ -956,11 +956,11 @@
       </c>
       <c r="H7" s="10">
         <f t="shared" si="3"/>
-        <v>83510.642857142855</v>
+        <v>73086.421052631573</v>
       </c>
       <c r="I7" s="10">
         <f t="shared" si="4"/>
-        <v>871016.005</v>
+        <v>665086.43157894723</v>
       </c>
       <c r="J7" s="10">
         <f t="shared" si="5"/>
@@ -973,18 +973,18 @@
       </c>
       <c r="M7" s="10">
         <f t="shared" si="7"/>
-        <v>9351.6957286834113</v>
+        <v>8175.2148828446952</v>
       </c>
       <c r="N7" s="9">
-        <v>10.43</v>
+        <v>9.1</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="9">
-        <v>8.93</v>
+        <v>8.94</v>
       </c>
       <c r="Q7" s="9"/>
       <c r="R7" s="12">
-        <v>0.74399999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="S7" s="12"/>
       <c r="T7" s="10">
@@ -996,12 +996,12 @@
         <v>0</v>
       </c>
       <c r="V7" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W7" s="9"/>
       <c r="X7" s="9">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1010,12 +1010,12 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10">
-        <v>2074085</v>
+        <v>1381714</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10">
         <f t="shared" si="0"/>
-        <v>2074085</v>
+        <v>1381714</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="1"/>
@@ -1027,11 +1027,11 @@
       </c>
       <c r="H8" s="10">
         <f t="shared" si="3"/>
-        <v>74074.46428571429</v>
+        <v>72721.789473684214</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="4"/>
-        <v>654818.26428571437</v>
+        <v>611590.24947368423</v>
       </c>
       <c r="J8" s="10">
         <f t="shared" si="5"/>
@@ -1044,18 +1044,18 @@
       </c>
       <c r="M8" s="10">
         <f t="shared" si="7"/>
-        <v>7520.2501812907913</v>
+        <v>7435.7657948552369</v>
       </c>
       <c r="N8" s="9">
-        <v>8.84</v>
+        <v>8.41</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9">
-        <v>9.85</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="12">
-        <v>0.68</v>
+        <v>0.68100000000000005</v>
       </c>
       <c r="S8" s="12"/>
       <c r="T8" s="10">
@@ -1067,12 +1067,12 @@
         <v>0</v>
       </c>
       <c r="V8" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W8" s="9"/>
       <c r="X8" s="9">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1081,12 +1081,12 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10">
-        <v>2929754</v>
+        <v>1855634</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>2929754</v>
+        <v>1855634</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="1"/>
@@ -1098,11 +1098,11 @@
       </c>
       <c r="H9" s="10">
         <f t="shared" si="3"/>
-        <v>104634.07142857143</v>
+        <v>97664.947368421053</v>
       </c>
       <c r="I9" s="10">
         <f t="shared" si="4"/>
-        <v>758597.01785714296</v>
+        <v>707094.21894736844</v>
       </c>
       <c r="J9" s="10">
         <f t="shared" si="5"/>
@@ -1115,14 +1115,14 @@
       </c>
       <c r="M9" s="10">
         <f t="shared" si="7"/>
-        <v>10622.748368382887</v>
+        <v>9986.1909374663664</v>
       </c>
       <c r="N9" s="9">
-        <v>7.25</v>
+        <v>7.24</v>
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="9">
-        <v>9.85</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="Q9" s="9"/>
       <c r="R9" s="12">
@@ -1138,12 +1138,12 @@
         <v>0</v>
       </c>
       <c r="V9" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W9" s="9"/>
       <c r="X9" s="9">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1152,12 +1152,12 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10">
-        <v>3414265</v>
+        <v>2526024</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>3414265</v>
+        <v>2526024</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="1"/>
@@ -1169,11 +1169,11 @@
       </c>
       <c r="H10" s="10">
         <f t="shared" si="3"/>
-        <v>121938.03571428571</v>
+        <v>132948.63157894736</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="4"/>
-        <v>1243767.9642857141</v>
+        <v>1261682.5136842104</v>
       </c>
       <c r="J10" s="10">
         <f t="shared" si="5"/>
@@ -1186,18 +1186,18 @@
       </c>
       <c r="M10" s="10">
         <f t="shared" si="7"/>
-        <v>12379.49601160261</v>
+        <v>13593.929609299323</v>
       </c>
       <c r="N10" s="9">
-        <v>10.199999999999999</v>
+        <v>9.49</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="9">
-        <v>9.85</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="Q10" s="9"/>
       <c r="R10" s="12">
-        <v>0.65</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="S10" s="12"/>
       <c r="T10" s="10">
@@ -1209,12 +1209,12 @@
         <v>0</v>
       </c>
       <c r="V10" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W10" s="9"/>
       <c r="X10" s="9">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1224,7 +1224,7 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8">
         <f t="shared" ref="C11:G11" si="11">SUM(C4:C10)</f>
-        <v>17096816</v>
+        <v>11297619</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="11"/>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="E11" s="8">
         <f t="shared" si="11"/>
-        <v>17096816</v>
+        <v>11297619</v>
       </c>
       <c r="F11" s="8">
         <f t="shared" si="11"/>
@@ -1244,11 +1244,11 @@
       </c>
       <c r="H11" s="8">
         <f>(E11+B11)/(X11+1)</f>
-        <v>610600.57142857148</v>
+        <v>594611.52631578944</v>
       </c>
       <c r="I11" s="8">
         <f t="shared" si="4"/>
-        <v>5019136.6971428581</v>
+        <v>4649862.1357894735</v>
       </c>
       <c r="J11" s="8">
         <f>B11*O11</f>
@@ -1261,14 +1261,14 @@
       </c>
       <c r="M11" s="8">
         <f t="shared" si="7"/>
-        <v>62625.699633699638</v>
+        <v>60798.724572166611</v>
       </c>
       <c r="N11" s="7">
-        <v>8.2200000000000006</v>
+        <v>7.82</v>
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7">
-        <v>9.75</v>
+        <v>9.7799999999999994</v>
       </c>
       <c r="Q11" s="7" t="e">
         <f>AVERAGE(Q4:Q10)</f>
@@ -1287,12 +1287,12 @@
         <v>0</v>
       </c>
       <c r="V11" s="7">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W11" s="7"/>
       <c r="X11" s="7">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1301,12 +1301,12 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10">
-        <v>3672922</v>
+        <v>2941602</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10">
         <f t="shared" si="0"/>
-        <v>3672922</v>
+        <v>2941602</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="1"/>
@@ -1318,11 +1318,11 @@
       </c>
       <c r="H12" s="10">
         <f t="shared" si="3"/>
-        <v>136034.14814814815</v>
+        <v>154821.15789473685</v>
       </c>
       <c r="I12" s="10">
         <f t="shared" si="4"/>
-        <v>560460.6903703704</v>
+        <v>574386.49578947376</v>
       </c>
       <c r="J12" s="10">
         <f t="shared" si="5"/>
@@ -1335,10 +1335,10 @@
       </c>
       <c r="M12" s="10">
         <f t="shared" si="7"/>
-        <v>12366.740740740741</v>
+        <v>14074.650717703351</v>
       </c>
       <c r="N12" s="9">
-        <v>4.12</v>
+        <v>3.71</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="Q12" s="9"/>
       <c r="R12" s="12">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="S12" s="12"/>
       <c r="T12" s="10">
@@ -1358,12 +1358,12 @@
         <v>0</v>
       </c>
       <c r="V12" s="9">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="W12" s="9"/>
       <c r="X12" s="9">
         <f t="shared" si="10"/>
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1372,12 +1372,12 @@
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10">
-        <v>800312</v>
+        <v>523283</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10">
         <f t="shared" si="0"/>
-        <v>800312</v>
+        <v>523283</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="1"/>
@@ -1389,11 +1389,11 @@
       </c>
       <c r="H13" s="10">
         <f t="shared" si="3"/>
-        <v>28582.571428571428</v>
+        <v>27541.21052631579</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="4"/>
-        <v>128621.57142857142</v>
+        <v>123935.44736842105</v>
       </c>
       <c r="J13" s="18">
         <f t="shared" si="5"/>
@@ -1406,14 +1406,14 @@
       </c>
       <c r="M13" s="10">
         <f t="shared" si="7"/>
-        <v>2901.7839013778098</v>
+        <v>2784.7533393645895</v>
       </c>
       <c r="N13" s="9">
         <v>4.5</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9">
-        <v>9.85</v>
+        <v>9.89</v>
       </c>
       <c r="Q13" s="9"/>
       <c r="R13" s="12">
@@ -1429,12 +1429,12 @@
         <v>0</v>
       </c>
       <c r="V13" s="9">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="W13" s="9"/>
       <c r="X13" s="9">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1446,13 +1446,15 @@
       <c r="E15" s="2"/>
       <c r="F15" s="1"/>
       <c r="I15" s="2"/>
+      <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -1471,11 +1473,12 @@
       <c r="F17" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <f>C11</f>
-        <v>17096816</v>
+        <v>11297619</v>
       </c>
       <c r="B18" s="14">
         <f>D11</f>
@@ -1495,10 +1498,11 @@
       </c>
       <c r="F18" s="14">
         <f>$C$11-E18</f>
-        <v>17096816</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11297619</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>43</v>
       </c>
@@ -1509,18 +1513,19 @@
       </c>
       <c r="D19" s="14">
         <f t="shared" ref="D19:D23" si="12">C19*$X$11</f>
-        <v>945000</v>
+        <v>630000</v>
       </c>
       <c r="E19" s="14">
         <f t="shared" ref="E19:E23" si="13">$D$11+D19</f>
-        <v>945000</v>
+        <v>630000</v>
       </c>
       <c r="F19" s="14">
         <f t="shared" ref="F19:F23" si="14">$C$11-E19</f>
-        <v>16151816</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10667619</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>43</v>
       </c>
@@ -1531,18 +1536,18 @@
       </c>
       <c r="D20" s="14">
         <f t="shared" si="12"/>
-        <v>1890000</v>
+        <v>1260000</v>
       </c>
       <c r="E20" s="14">
         <f t="shared" si="13"/>
-        <v>1890000</v>
+        <v>1260000</v>
       </c>
       <c r="F20" s="14">
         <f t="shared" si="14"/>
-        <v>15206816</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10037619</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>43</v>
       </c>
@@ -1553,18 +1558,18 @@
       </c>
       <c r="D21" s="14">
         <f t="shared" si="12"/>
-        <v>2835000</v>
+        <v>1890000</v>
       </c>
       <c r="E21" s="14">
         <f t="shared" si="13"/>
-        <v>2835000</v>
+        <v>1890000</v>
       </c>
       <c r="F21" s="14">
         <f t="shared" si="14"/>
-        <v>14261816</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9407619</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>43</v>
       </c>
@@ -1575,18 +1580,18 @@
       </c>
       <c r="D22" s="14">
         <f t="shared" si="12"/>
-        <v>3780000</v>
+        <v>2520000</v>
       </c>
       <c r="E22" s="14">
         <f t="shared" si="13"/>
-        <v>3780000</v>
+        <v>2520000</v>
       </c>
       <c r="F22" s="14">
         <f t="shared" si="14"/>
-        <v>13316816</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8777619</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>43</v>
       </c>
@@ -1597,15 +1602,15 @@
       </c>
       <c r="D23" s="14">
         <f t="shared" si="12"/>
-        <v>4725000</v>
+        <v>3150000</v>
       </c>
       <c r="E23" s="14">
         <f t="shared" si="13"/>
-        <v>4725000</v>
+        <v>3150000</v>
       </c>
       <c r="F23" s="14">
         <f t="shared" si="14"/>
-        <v>12371816</v>
+        <v>8147619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new Excel file with multiple worksheets and styles
- Created a new Excel file named "30-Jun-25.xlsx"
- Added multiple worksheets including a theme and styles
- Included document properties and core metadata
- The file contains a significant amount of data (8445 lines)
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Production follow up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6FB6D6-5CB7-441A-A5FC-13385AE2D0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A493F9-65D7-4817-8160-8B7AE1FA3394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Production Unit</t>
   </si>
@@ -135,9 +135,6 @@
     <t>JAL3</t>
   </si>
   <si>
-    <t>GTAL</t>
-  </si>
-  <si>
     <t>Plan vs Achievement</t>
   </si>
   <si>
@@ -166,6 +163,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>GTAL-LIN</t>
+  </si>
+  <si>
+    <t>GTAL-RMG</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +240,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -252,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -290,12 +299,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA4A4A4"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA4A4A4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -325,6 +345,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,16 +632,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X23"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
@@ -627,23 +651,23 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.42578125" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5">
         <f ca="1">TODAY() - 1</f>
-        <v>45809</v>
+        <v>45840</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -726,12 +750,12 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10">
-        <v>1827707</v>
+        <v>2143885</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10">
         <f>C4-D4</f>
-        <v>1827707</v>
+        <v>2143885</v>
       </c>
       <c r="F4" s="10">
         <f>C4*W4/V4</f>
@@ -743,11 +767,11 @@
       </c>
       <c r="H4" s="10">
         <f>(E4+B4)/(X4+1)</f>
-        <v>96195.105263157893</v>
+        <v>76567.321428571435</v>
       </c>
       <c r="I4" s="10">
         <f>H4*N4</f>
-        <v>662784.27526315791</v>
+        <v>576551.93035714293</v>
       </c>
       <c r="J4" s="10">
         <f>B4*O4</f>
@@ -760,18 +784,18 @@
       </c>
       <c r="M4" s="10">
         <f>H4/P4</f>
-        <v>9835.9003336562273</v>
+        <v>7656.7321428571431</v>
       </c>
       <c r="N4" s="9">
-        <v>6.89</v>
+        <v>7.53</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9">
-        <v>9.7799999999999994</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="9"/>
       <c r="R4" s="12">
-        <v>0.69</v>
+        <v>0.67</v>
       </c>
       <c r="S4" s="12"/>
       <c r="T4" s="10">
@@ -783,12 +807,12 @@
         <v>0</v>
       </c>
       <c r="V4" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9">
         <f>V4-W4</f>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -797,69 +821,69 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10">
-        <v>221717</v>
+        <v>262272</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10">
-        <f t="shared" ref="E5:E13" si="0">C5-D5</f>
-        <v>221717</v>
+        <f t="shared" ref="E5:E14" si="0">C5-D5</f>
+        <v>262272</v>
       </c>
       <c r="F5" s="10">
-        <f t="shared" ref="F5:F13" si="1">C5*W5/V5</f>
+        <f t="shared" ref="F5:F14" si="1">C5*W5/V5</f>
         <v>0</v>
       </c>
       <c r="G5" s="10">
-        <f t="shared" ref="G5:G13" si="2">F5-D5</f>
+        <f t="shared" ref="G5:G14" si="2">F5-D5</f>
         <v>0</v>
       </c>
       <c r="H5" s="10">
-        <f t="shared" ref="H5:H13" si="3">(E5+B5)/(X5+1)</f>
-        <v>11669.315789473685</v>
+        <f t="shared" ref="H5:H14" si="3">(E5+B5)/(X5+1)</f>
+        <v>9366.8571428571431</v>
       </c>
       <c r="I5" s="10">
-        <f t="shared" ref="I5:I13" si="4">H5*N5</f>
-        <v>73983.462105263156</v>
+        <f t="shared" ref="I5:I14" si="4">H5*N5</f>
+        <v>56950.491428571433</v>
       </c>
       <c r="J5" s="10">
-        <f t="shared" ref="J5:J13" si="5">B5*O5</f>
+        <f t="shared" ref="J5:J14" si="5">B5*O5</f>
         <v>0</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="17" t="e">
-        <f t="shared" ref="L5:L13" si="6">T5/U5</f>
+        <f t="shared" ref="L5:L14" si="6">T5/U5</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M5" s="18">
-        <f t="shared" ref="M5:M13" si="7">H5/P5</f>
-        <v>1193.1815735658165</v>
+        <f t="shared" ref="M5:M14" si="7">H5/P5</f>
+        <v>936.68571428571431</v>
       </c>
       <c r="N5" s="9">
-        <v>6.34</v>
+        <v>6.08</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9">
-        <v>9.7799999999999994</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="12">
-        <v>0.67</v>
+        <v>0.66</v>
       </c>
       <c r="S5" s="12"/>
       <c r="T5" s="10">
-        <f t="shared" ref="T5:T13" si="8">O5*D5</f>
+        <f t="shared" ref="T5:T14" si="8">O5*D5</f>
         <v>0</v>
       </c>
       <c r="U5" s="10">
-        <f t="shared" ref="U5:U13" si="9">N5*F5</f>
+        <f t="shared" ref="U5:U14" si="9">N5*F5</f>
         <v>0</v>
       </c>
       <c r="V5" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W5" s="9"/>
       <c r="X5" s="9">
-        <f t="shared" ref="X5:X13" si="10">V5-W5</f>
-        <v>18</v>
+        <f t="shared" ref="X5:X14" si="10">V5-W5</f>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -868,12 +892,12 @@
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10">
-        <v>2096181</v>
+        <v>1913112</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10">
         <f t="shared" si="0"/>
-        <v>2096181</v>
+        <v>1913112</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="1"/>
@@ -885,11 +909,11 @@
       </c>
       <c r="H6" s="10">
         <f t="shared" si="3"/>
-        <v>110325.31578947368</v>
+        <v>68325.428571428565</v>
       </c>
       <c r="I6" s="10">
         <f t="shared" si="4"/>
-        <v>692842.98315789469</v>
+        <v>426350.67428571428</v>
       </c>
       <c r="J6" s="10">
         <f t="shared" si="5"/>
@@ -902,18 +926,18 @@
       </c>
       <c r="M6" s="10">
         <f t="shared" si="7"/>
-        <v>10339.767178020027</v>
+        <v>6211.4025974025972</v>
       </c>
       <c r="N6" s="9">
-        <v>6.28</v>
+        <v>6.24</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="9">
-        <v>10.67</v>
+        <v>11</v>
       </c>
       <c r="Q6" s="9"/>
       <c r="R6" s="12">
-        <v>0.72399999999999998</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="S6" s="12"/>
       <c r="T6" s="10">
@@ -925,12 +949,12 @@
         <v>0</v>
       </c>
       <c r="V6" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W6" s="9"/>
       <c r="X6" s="9">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -939,12 +963,12 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10">
-        <v>1388642</v>
+        <v>2200195</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10">
         <f t="shared" si="0"/>
-        <v>1388642</v>
+        <v>2200195</v>
       </c>
       <c r="F7" s="10">
         <f t="shared" si="1"/>
@@ -956,11 +980,11 @@
       </c>
       <c r="H7" s="10">
         <f t="shared" si="3"/>
-        <v>73086.421052631573</v>
+        <v>78578.392857142855</v>
       </c>
       <c r="I7" s="10">
         <f t="shared" si="4"/>
-        <v>665086.43157894723</v>
+        <v>687560.9375</v>
       </c>
       <c r="J7" s="10">
         <f t="shared" si="5"/>
@@ -973,18 +997,18 @@
       </c>
       <c r="M7" s="10">
         <f t="shared" si="7"/>
-        <v>8175.2148828446952</v>
+        <v>8730.9325396825388</v>
       </c>
       <c r="N7" s="9">
-        <v>9.1</v>
+        <v>8.75</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="9">
-        <v>8.94</v>
+        <v>9</v>
       </c>
       <c r="Q7" s="9"/>
       <c r="R7" s="12">
-        <v>0.61</v>
+        <v>0.64200000000000002</v>
       </c>
       <c r="S7" s="12"/>
       <c r="T7" s="10">
@@ -996,12 +1020,12 @@
         <v>0</v>
       </c>
       <c r="V7" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W7" s="9"/>
       <c r="X7" s="9">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1010,12 +1034,12 @@
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10">
-        <v>1381714</v>
+        <v>2146320</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10">
         <f t="shared" si="0"/>
-        <v>1381714</v>
+        <v>2146320</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="1"/>
@@ -1027,11 +1051,11 @@
       </c>
       <c r="H8" s="10">
         <f t="shared" si="3"/>
-        <v>72721.789473684214</v>
+        <v>76654.28571428571</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="4"/>
-        <v>611590.24947368423</v>
+        <v>564942.08571428573</v>
       </c>
       <c r="J8" s="10">
         <f t="shared" si="5"/>
@@ -1044,18 +1068,18 @@
       </c>
       <c r="M8" s="10">
         <f t="shared" si="7"/>
-        <v>7435.7657948552369</v>
+        <v>7665.4285714285706</v>
       </c>
       <c r="N8" s="9">
-        <v>8.41</v>
+        <v>7.37</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9">
-        <v>9.7799999999999994</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="12">
-        <v>0.68100000000000005</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="S8" s="12"/>
       <c r="T8" s="10">
@@ -1067,12 +1091,12 @@
         <v>0</v>
       </c>
       <c r="V8" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W8" s="9"/>
       <c r="X8" s="9">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1081,12 +1105,12 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10">
-        <v>1855634</v>
+        <v>2342283</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>1855634</v>
+        <v>2342283</v>
       </c>
       <c r="F9" s="10">
         <f t="shared" si="1"/>
@@ -1098,11 +1122,11 @@
       </c>
       <c r="H9" s="10">
         <f t="shared" si="3"/>
-        <v>97664.947368421053</v>
+        <v>83652.96428571429</v>
       </c>
       <c r="I9" s="10">
         <f t="shared" si="4"/>
-        <v>707094.21894736844</v>
+        <v>683444.71821428579</v>
       </c>
       <c r="J9" s="10">
         <f t="shared" si="5"/>
@@ -1115,14 +1139,14 @@
       </c>
       <c r="M9" s="10">
         <f t="shared" si="7"/>
-        <v>9986.1909374663664</v>
+        <v>8365.2964285714297</v>
       </c>
       <c r="N9" s="9">
-        <v>7.24</v>
+        <v>8.17</v>
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="9">
-        <v>9.7799999999999994</v>
+        <v>10</v>
       </c>
       <c r="Q9" s="9"/>
       <c r="R9" s="12">
@@ -1138,12 +1162,12 @@
         <v>0</v>
       </c>
       <c r="V9" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W9" s="9"/>
       <c r="X9" s="9">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1152,12 +1176,12 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10">
-        <v>2526024</v>
+        <v>3425817</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10">
         <f t="shared" si="0"/>
-        <v>2526024</v>
+        <v>3425817</v>
       </c>
       <c r="F10" s="10">
         <f t="shared" si="1"/>
@@ -1169,11 +1193,11 @@
       </c>
       <c r="H10" s="10">
         <f t="shared" si="3"/>
-        <v>132948.63157894736</v>
+        <v>122350.60714285714</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="4"/>
-        <v>1261682.5136842104</v>
+        <v>1139084.1525000001</v>
       </c>
       <c r="J10" s="10">
         <f t="shared" si="5"/>
@@ -1186,18 +1210,18 @@
       </c>
       <c r="M10" s="10">
         <f t="shared" si="7"/>
-        <v>13593.929609299323</v>
+        <v>12235.060714285715</v>
       </c>
       <c r="N10" s="9">
-        <v>9.49</v>
+        <v>9.31</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="9">
-        <v>9.7799999999999994</v>
+        <v>10</v>
       </c>
       <c r="Q10" s="9"/>
       <c r="R10" s="12">
-        <v>0.65400000000000003</v>
+        <v>0.65</v>
       </c>
       <c r="S10" s="12"/>
       <c r="T10" s="10">
@@ -1209,12 +1233,12 @@
         <v>0</v>
       </c>
       <c r="V10" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W10" s="9"/>
       <c r="X10" s="9">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1223,32 +1247,32 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8">
-        <f t="shared" ref="C11:G11" si="11">SUM(C4:C10)</f>
-        <v>11297619</v>
+        <f>SUM(C4:C10)</f>
+        <v>14433884</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="11"/>
+        <f>SUM(D4:D10)</f>
         <v>0</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="11"/>
-        <v>11297619</v>
+        <f>SUM(E4:E10)</f>
+        <v>14433884</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="11"/>
+        <f>SUM(F4:F10)</f>
         <v>0</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" si="11"/>
+        <f>SUM(G4:G10)</f>
         <v>0</v>
       </c>
       <c r="H11" s="8">
         <f>(E11+B11)/(X11+1)</f>
-        <v>594611.52631578944</v>
+        <v>515495.85714285716</v>
       </c>
       <c r="I11" s="8">
         <f t="shared" si="4"/>
-        <v>4649862.1357894735</v>
+        <v>4108501.9814285715</v>
       </c>
       <c r="J11" s="8">
         <f>B11*O11</f>
@@ -1261,21 +1285,21 @@
       </c>
       <c r="M11" s="8">
         <f t="shared" si="7"/>
-        <v>60798.724572166611</v>
+        <v>51652.891497280274</v>
       </c>
       <c r="N11" s="7">
-        <v>7.82</v>
+        <v>7.97</v>
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7">
-        <v>9.7799999999999994</v>
+        <v>9.98</v>
       </c>
       <c r="Q11" s="7" t="e">
         <f>AVERAGE(Q4:Q10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="13">
-        <v>0.68620000000000003</v>
+        <v>0.66</v>
       </c>
       <c r="S11" s="13"/>
       <c r="T11" s="8">
@@ -1287,12 +1311,12 @@
         <v>0</v>
       </c>
       <c r="V11" s="7">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W11" s="7"/>
       <c r="X11" s="7">
         <f t="shared" si="10"/>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1301,12 +1325,12 @@
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10">
-        <v>2941602</v>
+        <v>3336041</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10">
         <f t="shared" si="0"/>
-        <v>2941602</v>
+        <v>3336041</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="1"/>
@@ -1318,11 +1342,11 @@
       </c>
       <c r="H12" s="10">
         <f t="shared" si="3"/>
-        <v>154821.15789473685</v>
+        <v>119144.32142857143</v>
       </c>
       <c r="I12" s="10">
         <f t="shared" si="4"/>
-        <v>574386.49578947376</v>
+        <v>442025.4325</v>
       </c>
       <c r="J12" s="10">
         <f t="shared" si="5"/>
@@ -1335,18 +1359,18 @@
       </c>
       <c r="M12" s="10">
         <f t="shared" si="7"/>
-        <v>14074.650717703351</v>
+        <v>13238.257936507936</v>
       </c>
       <c r="N12" s="9">
         <v>3.71</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="9">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q12" s="9"/>
       <c r="R12" s="12">
-        <v>0.81</v>
+        <v>0.78</v>
       </c>
       <c r="S12" s="12"/>
       <c r="T12" s="10">
@@ -1358,264 +1382,335 @@
         <v>0</v>
       </c>
       <c r="V12" s="9">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="W12" s="9"/>
       <c r="X12" s="9">
         <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10">
-        <v>523283</v>
+        <v>44</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19">
+        <v>959072</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10">
+        <f t="shared" ref="E13" si="11">C13-D13</f>
+        <v>959072</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" ref="F13" si="12">C13*W13/V13</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" ref="G13" si="13">F13-D13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" ref="H13" si="14">(E13+B13)/(X13+1)</f>
+        <v>34252.571428571428</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" ref="I13" si="15">H13*N13</f>
+        <v>233602.53714285715</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" ref="J13" si="16">B13*O13</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="17" t="e">
+        <f t="shared" ref="L13" si="17">T13/U13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="10">
+        <f t="shared" ref="M13" si="18">H13/P13</f>
+        <v>3425.2571428571428</v>
+      </c>
+      <c r="N13" s="22">
+        <v>6.82</v>
+      </c>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="21">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="S13" s="12"/>
+      <c r="T13" s="10">
+        <f t="shared" ref="T13" si="19">O13*D13</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="10">
+        <f t="shared" ref="U13" si="20">N13*F13</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="9">
+        <v>27</v>
+      </c>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9">
+        <f t="shared" ref="X13" si="21">V13-W13</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10">
         <f t="shared" si="0"/>
-        <v>523283</v>
-      </c>
-      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G14" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H14" s="10">
         <f t="shared" si="3"/>
-        <v>27541.21052631579</v>
-      </c>
-      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
         <f t="shared" si="4"/>
-        <v>123935.44736842105</v>
-      </c>
-      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J14" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="17" t="e">
+      <c r="K14" s="9"/>
+      <c r="L14" s="17" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M14" s="10">
         <f t="shared" si="7"/>
-        <v>2784.7533393645895</v>
-      </c>
-      <c r="N13" s="9">
-        <v>4.5</v>
-      </c>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9">
-        <v>9.89</v>
-      </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="12">
-        <v>0.65</v>
-      </c>
-      <c r="S13" s="12"/>
-      <c r="T13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N14" s="9">
+        <v>0</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="12">
+        <v>0</v>
+      </c>
+      <c r="S14" s="12"/>
+      <c r="T14" s="9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U13" s="10">
+      <c r="U14" s="10">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V13" s="9">
-        <v>18</v>
-      </c>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9">
+      <c r="V14" s="9">
+        <v>27</v>
+      </c>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9">
         <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-      <c r="I15" s="2"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
         <f>C11</f>
-        <v>11297619</v>
-      </c>
-      <c r="B18" s="14">
+        <v>14433884</v>
+      </c>
+      <c r="B19" s="14">
         <f>D11</f>
         <v>0</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C19" s="14">
         <f>QUOTIENT(B11,10000)*10000</f>
         <v>0</v>
       </c>
-      <c r="D18" s="14">
-        <f>C18*$X$11</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="14">
-        <f>$D$11+D18</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="14">
-        <f>$C$11-E18</f>
-        <v>11297619</v>
-      </c>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="14">
-        <f>C18+35000</f>
-        <v>35000</v>
-      </c>
       <c r="D19" s="14">
-        <f t="shared" ref="D19:D23" si="12">C19*$X$11</f>
-        <v>630000</v>
+        <f>C19*$X$11</f>
+        <v>0</v>
       </c>
       <c r="E19" s="14">
-        <f t="shared" ref="E19:E23" si="13">$D$11+D19</f>
-        <v>630000</v>
+        <f>$D$11+D19</f>
+        <v>0</v>
       </c>
       <c r="F19" s="14">
-        <f t="shared" ref="F19:F23" si="14">$C$11-E19</f>
-        <v>10667619</v>
+        <f>$C$11-E19</f>
+        <v>14433884</v>
       </c>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="14">
-        <f t="shared" ref="C20:C23" si="15">C19+35000</f>
-        <v>70000</v>
+        <f>C19+35000</f>
+        <v>35000</v>
       </c>
       <c r="D20" s="14">
-        <f t="shared" si="12"/>
-        <v>1260000</v>
+        <f t="shared" ref="D20:D24" si="22">C20*$X$11</f>
+        <v>945000</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" si="13"/>
-        <v>1260000</v>
+        <f t="shared" ref="E20:E24" si="23">$D$11+D20</f>
+        <v>945000</v>
       </c>
       <c r="F20" s="14">
-        <f t="shared" si="14"/>
-        <v>10037619</v>
-      </c>
+        <f t="shared" ref="F20:F24" si="24">$C$11-E20</f>
+        <v>13488884</v>
+      </c>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="14">
-        <f t="shared" si="15"/>
-        <v>105000</v>
+        <f t="shared" ref="C21:C24" si="25">C20+35000</f>
+        <v>70000</v>
       </c>
       <c r="D21" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="22"/>
         <v>1890000</v>
       </c>
       <c r="E21" s="14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="23"/>
         <v>1890000</v>
       </c>
       <c r="F21" s="14">
-        <f t="shared" si="14"/>
-        <v>9407619</v>
+        <f t="shared" si="24"/>
+        <v>12543884</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="14">
-        <f t="shared" si="15"/>
-        <v>140000</v>
+        <f t="shared" si="25"/>
+        <v>105000</v>
       </c>
       <c r="D22" s="14">
-        <f t="shared" si="12"/>
-        <v>2520000</v>
+        <f t="shared" si="22"/>
+        <v>2835000</v>
       </c>
       <c r="E22" s="14">
-        <f t="shared" si="13"/>
-        <v>2520000</v>
+        <f t="shared" si="23"/>
+        <v>2835000</v>
       </c>
       <c r="F22" s="14">
-        <f t="shared" si="14"/>
-        <v>8777619</v>
+        <f t="shared" si="24"/>
+        <v>11598884</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="25"/>
+        <v>140000</v>
+      </c>
+      <c r="D23" s="14">
+        <f t="shared" si="22"/>
+        <v>3780000</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" si="23"/>
+        <v>3780000</v>
+      </c>
+      <c r="F23" s="14">
+        <f t="shared" si="24"/>
+        <v>10653884</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="14">
+        <f t="shared" si="25"/>
         <v>175000</v>
       </c>
-      <c r="D23" s="14">
-        <f t="shared" si="12"/>
-        <v>3150000</v>
-      </c>
-      <c r="E23" s="14">
-        <f t="shared" si="13"/>
-        <v>3150000</v>
-      </c>
-      <c r="F23" s="14">
-        <f t="shared" si="14"/>
-        <v>8147619</v>
+      <c r="D24" s="14">
+        <f t="shared" si="22"/>
+        <v>4725000</v>
+      </c>
+      <c r="E24" s="14">
+        <f t="shared" si="23"/>
+        <v>4725000</v>
+      </c>
+      <c r="F24" s="14">
+        <f t="shared" si="24"/>
+        <v>9708884</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="K12:K13 K4:K10" name="otshedule24" securityDescriptor="O:WDG:WDD:(A;;CC;;;WD)"/>
+    <protectedRange sqref="K12:K14 K4:K10" name="otshedule24" securityDescriptor="O:WDG:WDD:(A;;CC;;;WD)"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated the prodcess to take data from .html file
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Production follow up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A493F9-65D7-4817-8160-8B7AE1FA3394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB138FE-9C68-4B3F-A5ED-96A5B07B0563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Production Unit</t>
   </si>
@@ -165,10 +165,7 @@
     <t>-</t>
   </si>
   <si>
-    <t>GTAL-LIN</t>
-  </si>
-  <si>
-    <t>GTAL-RMG</t>
+    <t>GTAL</t>
   </si>
 </sst>
 </file>
@@ -199,12 +196,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -245,6 +236,11 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Playfair Display"/>
     </font>
   </fonts>
   <fills count="3">
@@ -315,39 +311,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -632,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,1061 +651,990 @@
     <col min="21" max="21" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:24" ht="29.25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <f ca="1">TODAY() - 1</f>
-        <v>45840</v>
+        <v>45846</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="V3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="W3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="X3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9">
         <v>2143885</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9">
         <f>C4-D4</f>
         <v>2143885</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <f>C4*W4/V4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <f>F4-D4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <f>(E4+B4)/(X4+1)</f>
         <v>76567.321428571435</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <f>H4*N4</f>
         <v>576551.93035714293</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <f>B4*O4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="17" t="e">
+      <c r="K4" s="9"/>
+      <c r="L4" s="16" t="e">
         <f>T4/U4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <f>H4/P4</f>
         <v>7656.7321428571431</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="8">
         <v>7.53</v>
       </c>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9">
+      <c r="O4" s="8"/>
+      <c r="P4" s="8">
         <v>10</v>
       </c>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="12">
+      <c r="Q4" s="8"/>
+      <c r="R4" s="11">
         <v>0.67</v>
       </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="10">
+      <c r="S4" s="11"/>
+      <c r="T4" s="9">
         <f>O4*D4</f>
         <v>0</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U4" s="9">
         <f>N4*F4</f>
         <v>0</v>
       </c>
-      <c r="V4" s="9">
-        <v>27</v>
-      </c>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9">
+      <c r="V4" s="8">
+        <v>27</v>
+      </c>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8">
         <f>V4-W4</f>
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9">
         <v>262272</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10">
-        <f t="shared" ref="E5:E14" si="0">C5-D5</f>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
+        <f t="shared" ref="E5:E12" si="0">C5-D5</f>
         <v>262272</v>
       </c>
-      <c r="F5" s="10">
-        <f t="shared" ref="F5:F14" si="1">C5*W5/V5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="10">
-        <f t="shared" ref="G5:G14" si="2">F5-D5</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="10">
-        <f t="shared" ref="H5:H14" si="3">(E5+B5)/(X5+1)</f>
+      <c r="F5" s="9">
+        <f t="shared" ref="F5:F12" si="1">C5*W5/V5</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" ref="G5:G12" si="2">F5-D5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" ref="H5:H12" si="3">(E5+B5)/(X5+1)</f>
         <v>9366.8571428571431</v>
       </c>
-      <c r="I5" s="10">
-        <f t="shared" ref="I5:I14" si="4">H5*N5</f>
+      <c r="I5" s="9">
+        <f t="shared" ref="I5:I12" si="4">H5*N5</f>
         <v>56950.491428571433</v>
       </c>
-      <c r="J5" s="10">
-        <f t="shared" ref="J5:J14" si="5">B5*O5</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="17" t="e">
-        <f t="shared" ref="L5:L14" si="6">T5/U5</f>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:J12" si="5">B5*O5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="16" t="e">
+        <f t="shared" ref="L5:L12" si="6">T5/U5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M5" s="18">
-        <f t="shared" ref="M5:M14" si="7">H5/P5</f>
+      <c r="M5" s="17">
+        <f t="shared" ref="M5:M12" si="7">H5/P5</f>
         <v>936.68571428571431</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <v>6.08</v>
       </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9">
+      <c r="O5" s="8"/>
+      <c r="P5" s="8">
         <v>10</v>
       </c>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="12">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="11">
         <v>0.66</v>
       </c>
-      <c r="S5" s="12"/>
-      <c r="T5" s="10">
-        <f t="shared" ref="T5:T14" si="8">O5*D5</f>
-        <v>0</v>
-      </c>
-      <c r="U5" s="10">
-        <f t="shared" ref="U5:U14" si="9">N5*F5</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="9">
-        <v>27</v>
-      </c>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9">
-        <f t="shared" ref="X5:X14" si="10">V5-W5</f>
+      <c r="S5" s="11"/>
+      <c r="T5" s="9">
+        <f t="shared" ref="T5:T12" si="8">O5*D5</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="9">
+        <f t="shared" ref="U5:U12" si="9">N5*F5</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="8">
+        <v>27</v>
+      </c>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8">
+        <f t="shared" ref="X5:X12" si="10">V5-W5</f>
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
         <v>1913112</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
         <f t="shared" si="0"/>
         <v>1913112</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <f t="shared" si="3"/>
         <v>68325.428571428565</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <f t="shared" si="4"/>
         <v>426350.67428571428</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="17" t="e">
+      <c r="K6" s="9"/>
+      <c r="L6" s="16" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <f t="shared" si="7"/>
         <v>6211.4025974025972</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="8">
         <v>6.24</v>
       </c>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9">
+      <c r="O6" s="8"/>
+      <c r="P6" s="8">
         <v>11</v>
       </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="12">
+      <c r="Q6" s="8"/>
+      <c r="R6" s="11">
         <v>0.72799999999999998</v>
       </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="10">
+      <c r="S6" s="11"/>
+      <c r="T6" s="9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U6" s="10">
+      <c r="U6" s="9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V6" s="9">
-        <v>27</v>
-      </c>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9">
+      <c r="V6" s="8">
+        <v>27</v>
+      </c>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9">
         <v>2200195</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
         <f t="shared" si="0"/>
         <v>2200195</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <f t="shared" si="3"/>
         <v>78578.392857142855</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <f t="shared" si="4"/>
         <v>687560.9375</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="17" t="e">
+      <c r="K7" s="9"/>
+      <c r="L7" s="16" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <f t="shared" si="7"/>
         <v>8730.9325396825388</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="8">
         <v>8.75</v>
       </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9">
+      <c r="O7" s="8"/>
+      <c r="P7" s="8">
         <v>9</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="12">
+      <c r="Q7" s="8"/>
+      <c r="R7" s="11">
         <v>0.64200000000000002</v>
       </c>
-      <c r="S7" s="12"/>
-      <c r="T7" s="10">
+      <c r="S7" s="11"/>
+      <c r="T7" s="9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U7" s="10">
+      <c r="U7" s="9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V7" s="9">
-        <v>27</v>
-      </c>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9">
+      <c r="V7" s="8">
+        <v>27</v>
+      </c>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9">
         <v>2146320</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <f t="shared" si="0"/>
         <v>2146320</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <f t="shared" si="3"/>
         <v>76654.28571428571</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <f t="shared" si="4"/>
         <v>564942.08571428573</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="17" t="e">
+      <c r="K8" s="9"/>
+      <c r="L8" s="16" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <f t="shared" si="7"/>
         <v>7665.4285714285706</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="8">
         <v>7.37</v>
       </c>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9">
+      <c r="O8" s="8"/>
+      <c r="P8" s="8">
         <v>10</v>
       </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="12">
+      <c r="Q8" s="8"/>
+      <c r="R8" s="11">
         <v>0.66200000000000003</v>
       </c>
-      <c r="S8" s="12"/>
-      <c r="T8" s="10">
+      <c r="S8" s="11"/>
+      <c r="T8" s="9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U8" s="10">
+      <c r="U8" s="9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V8" s="9">
-        <v>27</v>
-      </c>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9">
+      <c r="V8" s="8">
+        <v>27</v>
+      </c>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9">
         <v>2342283</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
         <f t="shared" si="0"/>
         <v>2342283</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <f t="shared" si="3"/>
         <v>83652.96428571429</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <f t="shared" si="4"/>
         <v>683444.71821428579</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="17" t="e">
+      <c r="K9" s="9"/>
+      <c r="L9" s="16" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="9">
         <f t="shared" si="7"/>
         <v>8365.2964285714297</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="8">
         <v>8.17</v>
       </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9">
+      <c r="O9" s="8"/>
+      <c r="P9" s="8">
         <v>10</v>
       </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="12">
+      <c r="Q9" s="8"/>
+      <c r="R9" s="11">
         <v>0.68</v>
       </c>
-      <c r="S9" s="12"/>
-      <c r="T9" s="10">
+      <c r="S9" s="11"/>
+      <c r="T9" s="9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U9" s="10">
+      <c r="U9" s="9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V9" s="9">
-        <v>27</v>
-      </c>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9">
+      <c r="V9" s="8">
+        <v>27</v>
+      </c>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9">
         <v>3425817</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
         <f t="shared" si="0"/>
         <v>3425817</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <f t="shared" si="3"/>
         <v>122350.60714285714</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <f t="shared" si="4"/>
         <v>1139084.1525000001</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="17" t="e">
+      <c r="K10" s="9"/>
+      <c r="L10" s="16" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <f t="shared" si="7"/>
         <v>12235.060714285715</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="8">
         <v>9.31</v>
       </c>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9">
+      <c r="O10" s="8"/>
+      <c r="P10" s="8">
         <v>10</v>
       </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="12">
+      <c r="Q10" s="8"/>
+      <c r="R10" s="11">
         <v>0.65</v>
       </c>
-      <c r="S10" s="12"/>
-      <c r="T10" s="10">
+      <c r="S10" s="11"/>
+      <c r="T10" s="9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U10" s="10">
+      <c r="U10" s="9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V10" s="9">
-        <v>27</v>
-      </c>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9">
+      <c r="V10" s="8">
+        <v>27</v>
+      </c>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7">
         <f>SUM(C4:C10)</f>
         <v>14433884</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <f>SUM(D4:D10)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <f>SUM(E4:E10)</f>
         <v>14433884</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <f>SUM(F4:F10)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <f>SUM(G4:G10)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <f>(E11+B11)/(X11+1)</f>
         <v>515495.85714285716</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <f t="shared" si="4"/>
         <v>4108501.9814285715</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <f>B11*O11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="8"/>
-      <c r="L11" s="13" t="e">
+      <c r="K11" s="7"/>
+      <c r="L11" s="12" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11" s="7">
         <f t="shared" si="7"/>
         <v>51652.891497280274</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="6">
         <v>7.97</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7">
+      <c r="O11" s="6"/>
+      <c r="P11" s="6">
         <v>9.98</v>
       </c>
-      <c r="Q11" s="7" t="e">
+      <c r="Q11" s="6" t="e">
         <f>AVERAGE(Q4:Q10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R11" s="13">
-        <v>0.66</v>
-      </c>
-      <c r="S11" s="13"/>
-      <c r="T11" s="8">
+      <c r="R11" s="12">
+        <v>0.67</v>
+      </c>
+      <c r="S11" s="12"/>
+      <c r="T11" s="7">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U11" s="8">
+      <c r="U11" s="7">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V11" s="7">
-        <v>27</v>
-      </c>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7">
+      <c r="V11" s="6">
+        <v>27</v>
+      </c>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9">
         <v>3336041</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
         <f t="shared" si="0"/>
         <v>3336041</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <f t="shared" si="3"/>
         <v>119144.32142857143</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <f t="shared" si="4"/>
-        <v>442025.4325</v>
-      </c>
-      <c r="J12" s="10">
+        <v>427728.11392857146</v>
+      </c>
+      <c r="J12" s="9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="17" t="e">
+      <c r="K12" s="9"/>
+      <c r="L12" s="16" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="9">
         <f t="shared" si="7"/>
         <v>13238.257936507936</v>
       </c>
-      <c r="N12" s="9">
-        <v>3.71</v>
-      </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9">
+      <c r="N12" s="8">
+        <v>3.59</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8">
         <v>9</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="12">
+      <c r="Q12" s="8"/>
+      <c r="R12" s="11">
         <v>0.78</v>
       </c>
-      <c r="S12" s="12"/>
-      <c r="T12" s="10">
+      <c r="S12" s="11"/>
+      <c r="T12" s="9">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U12" s="10">
+      <c r="U12" s="9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V12" s="9">
-        <v>27</v>
-      </c>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9">
+      <c r="V12" s="8">
+        <v>27</v>
+      </c>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8">
         <f t="shared" si="10"/>
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19">
+      <c r="A13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9">
         <v>959072</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
         <f t="shared" ref="E13" si="11">C13-D13</f>
         <v>959072</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <f t="shared" ref="F13" si="12">C13*W13/V13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <f t="shared" ref="G13" si="13">F13-D13</f>
         <v>0</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <f t="shared" ref="H13" si="14">(E13+B13)/(X13+1)</f>
         <v>34252.571428571428</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <f t="shared" ref="I13" si="15">H13*N13</f>
         <v>233602.53714285715</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <f t="shared" ref="J13" si="16">B13*O13</f>
         <v>0</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="17" t="e">
+      <c r="K13" s="9"/>
+      <c r="L13" s="16" t="e">
         <f t="shared" ref="L13" si="17">T13/U13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="9">
         <f t="shared" ref="M13" si="18">H13/P13</f>
         <v>3425.2571428571428</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="20">
         <v>6.82</v>
       </c>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20">
+      <c r="O13" s="18"/>
+      <c r="P13" s="18">
         <v>10</v>
       </c>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="21">
+      <c r="Q13" s="18"/>
+      <c r="R13" s="19">
         <v>0.61799999999999999</v>
       </c>
-      <c r="S13" s="12"/>
-      <c r="T13" s="10">
+      <c r="S13" s="11"/>
+      <c r="T13" s="9">
         <f t="shared" ref="T13" si="19">O13*D13</f>
         <v>0</v>
       </c>
-      <c r="U13" s="10">
+      <c r="U13" s="9">
         <f t="shared" ref="U13" si="20">N13*F13</f>
         <v>0</v>
       </c>
-      <c r="V13" s="9">
-        <v>27</v>
-      </c>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9">
+      <c r="V13" s="8">
+        <v>27</v>
+      </c>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8">
         <f t="shared" ref="X13" si="21">V13-W13</f>
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10">
-        <v>0</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="18">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="17" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="9">
-        <v>0</v>
-      </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9">
-        <v>10</v>
-      </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="12">
-        <v>0</v>
-      </c>
-      <c r="S14" s="12"/>
-      <c r="T14" s="9">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U14" s="10">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="9">
-        <v>27</v>
-      </c>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9">
-        <f t="shared" si="10"/>
-        <v>27</v>
-      </c>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="1"/>
-      <c r="I16" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <f>C11</f>
         <v>14433884</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B18" s="13">
         <f>D11</f>
         <v>0</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C18" s="13">
         <f>QUOTIENT(B11,10000)*10000</f>
         <v>0</v>
       </c>
-      <c r="D19" s="14">
-        <f>C19*$X$11</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="14">
-        <f>$D$11+D19</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="14">
-        <f>$C$11-E19</f>
+      <c r="D18" s="13">
+        <f>C18*$X$11</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="13">
+        <f>$D$11+D18</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="13">
+        <f>$C$11-E18</f>
         <v>14433884</v>
       </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="13">
+        <f>C18+35000</f>
+        <v>35000</v>
+      </c>
+      <c r="D19" s="13">
+        <f t="shared" ref="D19:D23" si="22">C19*$X$11</f>
+        <v>945000</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" ref="E19:E23" si="23">$D$11+D19</f>
+        <v>945000</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" ref="F19:F23" si="24">$C$11-E19</f>
+        <v>13488884</v>
+      </c>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="14">
-        <f>C19+35000</f>
-        <v>35000</v>
-      </c>
-      <c r="D20" s="14">
-        <f t="shared" ref="D20:D24" si="22">C20*$X$11</f>
-        <v>945000</v>
-      </c>
-      <c r="E20" s="14">
-        <f t="shared" ref="E20:E24" si="23">$D$11+D20</f>
-        <v>945000</v>
-      </c>
-      <c r="F20" s="14">
-        <f t="shared" ref="F20:F24" si="24">$C$11-E20</f>
-        <v>13488884</v>
-      </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="14">
-        <f t="shared" ref="C21:C24" si="25">C20+35000</f>
+      <c r="B20" s="14"/>
+      <c r="C20" s="13">
+        <f t="shared" ref="C20:C23" si="25">C19+35000</f>
         <v>70000</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D20" s="13">
         <f t="shared" si="22"/>
         <v>1890000</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E20" s="13">
         <f t="shared" si="23"/>
         <v>1890000</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F20" s="13">
         <f t="shared" si="24"/>
         <v>12543884</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="14">
+      <c r="B21" s="14"/>
+      <c r="C21" s="13">
         <f t="shared" si="25"/>
         <v>105000</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D21" s="13">
         <f t="shared" si="22"/>
         <v>2835000</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E21" s="13">
         <f t="shared" si="23"/>
         <v>2835000</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F21" s="13">
         <f t="shared" si="24"/>
         <v>11598884</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="14">
+      <c r="B22" s="14"/>
+      <c r="C22" s="13">
         <f t="shared" si="25"/>
         <v>140000</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D22" s="13">
         <f t="shared" si="22"/>
         <v>3780000</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E22" s="13">
         <f t="shared" si="23"/>
         <v>3780000</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F22" s="13">
         <f t="shared" si="24"/>
         <v>10653884</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="14">
+      <c r="B23" s="14"/>
+      <c r="C23" s="13">
         <f t="shared" si="25"/>
         <v>175000</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D23" s="13">
         <f t="shared" si="22"/>
         <v>4725000</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E23" s="13">
         <f t="shared" si="23"/>
         <v>4725000</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F23" s="13">
         <f t="shared" si="24"/>
         <v>9708884</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="K12:K14 K4:K10" name="otshedule24" securityDescriptor="O:WDG:WDD:(A;;CC;;;WD)"/>
+    <protectedRange sqref="K4:K10 K12:K13" name="otshedule24" securityDescriptor="O:WDG:WDD:(A;;CC;;;WD)"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated for the month of august
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Production follow up\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Work\1. Daily\Production follow up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB138FE-9C68-4B3F-A5ED-96A5B07B0563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40213D5-7C43-4AD8-B313-70FC50927103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,7 +630,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +662,7 @@
       </c>
       <c r="B2" s="4">
         <f ca="1">TODAY() - 1</f>
-        <v>45846</v>
+        <v>45871</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -745,12 +745,12 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9">
-        <v>2143885</v>
+        <v>1688592</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9">
         <f>C4-D4</f>
-        <v>2143885</v>
+        <v>1688592</v>
       </c>
       <c r="F4" s="9">
         <f>C4*W4/V4</f>
@@ -762,11 +762,11 @@
       </c>
       <c r="H4" s="9">
         <f>(E4+B4)/(X4+1)</f>
-        <v>76567.321428571435</v>
+        <v>62540.444444444445</v>
       </c>
       <c r="I4" s="9">
         <f>H4*N4</f>
-        <v>576551.93035714293</v>
+        <v>506577.6</v>
       </c>
       <c r="J4" s="9">
         <f>B4*O4</f>
@@ -779,18 +779,18 @@
       </c>
       <c r="M4" s="9">
         <f>H4/P4</f>
-        <v>7656.7321428571431</v>
+        <v>6948.9382716049386</v>
       </c>
       <c r="N4" s="8">
-        <v>7.53</v>
+        <v>8.1</v>
       </c>
       <c r="O4" s="8"/>
       <c r="P4" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="11">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="S4" s="11"/>
       <c r="T4" s="9">
@@ -802,12 +802,12 @@
         <v>0</v>
       </c>
       <c r="V4" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W4" s="8"/>
       <c r="X4" s="8">
         <f>V4-W4</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -816,12 +816,12 @@
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9">
-        <v>262272</v>
+        <v>206218</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9">
         <f t="shared" ref="E5:E12" si="0">C5-D5</f>
-        <v>262272</v>
+        <v>206218</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" ref="F5:F12" si="1">C5*W5/V5</f>
@@ -833,11 +833,11 @@
       </c>
       <c r="H5" s="9">
         <f t="shared" ref="H5:H12" si="3">(E5+B5)/(X5+1)</f>
-        <v>9366.8571428571431</v>
+        <v>7637.7037037037035</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" ref="I5:I12" si="4">H5*N5</f>
-        <v>56950.491428571433</v>
+        <v>61865.399999999994</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" ref="J5:J12" si="5">B5*O5</f>
@@ -850,18 +850,18 @@
       </c>
       <c r="M5" s="17">
         <f t="shared" ref="M5:M12" si="7">H5/P5</f>
-        <v>936.68571428571431</v>
+        <v>848.63374485596705</v>
       </c>
       <c r="N5" s="8">
-        <v>6.08</v>
+        <v>8.1</v>
       </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="11">
-        <v>0.66</v>
+        <v>0.68</v>
       </c>
       <c r="S5" s="11"/>
       <c r="T5" s="9">
@@ -873,12 +873,12 @@
         <v>0</v>
       </c>
       <c r="V5" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W5" s="8"/>
       <c r="X5" s="8">
         <f t="shared" ref="X5:X12" si="10">V5-W5</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -887,12 +887,12 @@
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9">
-        <v>1913112</v>
+        <v>1226090</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9">
         <f t="shared" si="0"/>
-        <v>1913112</v>
+        <v>1226090</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="1"/>
@@ -904,11 +904,11 @@
       </c>
       <c r="H6" s="9">
         <f t="shared" si="3"/>
-        <v>68325.428571428565</v>
+        <v>45410.740740740737</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" si="4"/>
-        <v>426350.67428571428</v>
+        <v>327865.54814814811</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" si="5"/>
@@ -921,18 +921,18 @@
       </c>
       <c r="M6" s="9">
         <f t="shared" si="7"/>
-        <v>6211.4025974025972</v>
+        <v>4541.0740740740739</v>
       </c>
       <c r="N6" s="8">
-        <v>6.24</v>
+        <v>7.22</v>
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="11">
-        <v>0.72799999999999998</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="S6" s="11"/>
       <c r="T6" s="9">
@@ -944,12 +944,12 @@
         <v>0</v>
       </c>
       <c r="V6" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -958,12 +958,12 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9">
-        <v>2200195</v>
+        <v>1844988</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9">
         <f t="shared" si="0"/>
-        <v>2200195</v>
+        <v>1844988</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
@@ -975,11 +975,11 @@
       </c>
       <c r="H7" s="9">
         <f t="shared" si="3"/>
-        <v>78578.392857142855</v>
+        <v>68332.888888888891</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" si="4"/>
-        <v>687560.9375</v>
+        <v>557596.37333333341</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" si="5"/>
@@ -992,18 +992,18 @@
       </c>
       <c r="M7" s="9">
         <f t="shared" si="7"/>
-        <v>8730.9325396825388</v>
+        <v>8541.6111111111113</v>
       </c>
       <c r="N7" s="8">
-        <v>8.75</v>
+        <v>8.16</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="11">
-        <v>0.64200000000000002</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="9">
@@ -1015,12 +1015,12 @@
         <v>0</v>
       </c>
       <c r="V7" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1029,12 +1029,12 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9">
-        <v>2146320</v>
+        <v>2255336</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9">
         <f t="shared" si="0"/>
-        <v>2146320</v>
+        <v>2255336</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="1"/>
@@ -1046,11 +1046,11 @@
       </c>
       <c r="H8" s="9">
         <f t="shared" si="3"/>
-        <v>76654.28571428571</v>
+        <v>83530.962962962964</v>
       </c>
       <c r="I8" s="9">
         <f t="shared" si="4"/>
-        <v>564942.08571428573</v>
+        <v>610611.33925925929</v>
       </c>
       <c r="J8" s="9">
         <f t="shared" si="5"/>
@@ -1063,10 +1063,10 @@
       </c>
       <c r="M8" s="9">
         <f t="shared" si="7"/>
-        <v>7665.4285714285706</v>
+        <v>8353.0962962962967</v>
       </c>
       <c r="N8" s="8">
-        <v>7.37</v>
+        <v>7.31</v>
       </c>
       <c r="O8" s="8"/>
       <c r="P8" s="8">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="11">
-        <v>0.66200000000000003</v>
+        <v>0.65</v>
       </c>
       <c r="S8" s="11"/>
       <c r="T8" s="9">
@@ -1086,12 +1086,12 @@
         <v>0</v>
       </c>
       <c r="V8" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1100,12 +1100,12 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9">
-        <v>2342283</v>
+        <v>1365460</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9">
         <f t="shared" si="0"/>
-        <v>2342283</v>
+        <v>1365460</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="1"/>
@@ -1117,11 +1117,11 @@
       </c>
       <c r="H9" s="9">
         <f t="shared" si="3"/>
-        <v>83652.96428571429</v>
+        <v>50572.592592592591</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="4"/>
-        <v>683444.71821428579</v>
+        <v>380305.89629629627</v>
       </c>
       <c r="J9" s="9">
         <f t="shared" si="5"/>
@@ -1134,14 +1134,14 @@
       </c>
       <c r="M9" s="9">
         <f t="shared" si="7"/>
-        <v>8365.2964285714297</v>
+        <v>6321.5740740740739</v>
       </c>
       <c r="N9" s="8">
-        <v>8.17</v>
+        <v>7.52</v>
       </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="8"/>
       <c r="R9" s="11">
@@ -1157,12 +1157,12 @@
         <v>0</v>
       </c>
       <c r="V9" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1171,12 +1171,12 @@
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9">
-        <v>3425817</v>
+        <v>2667920</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9">
         <f t="shared" si="0"/>
-        <v>3425817</v>
+        <v>2667920</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
@@ -1188,11 +1188,11 @@
       </c>
       <c r="H10" s="9">
         <f t="shared" si="3"/>
-        <v>122350.60714285714</v>
+        <v>98811.851851851854</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" si="4"/>
-        <v>1139084.1525000001</v>
+        <v>929819.52592592593</v>
       </c>
       <c r="J10" s="9">
         <f t="shared" si="5"/>
@@ -1205,18 +1205,18 @@
       </c>
       <c r="M10" s="9">
         <f t="shared" si="7"/>
-        <v>12235.060714285715</v>
+        <v>12351.481481481482</v>
       </c>
       <c r="N10" s="8">
-        <v>9.31</v>
+        <v>9.41</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="11">
-        <v>0.65</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="S10" s="11"/>
       <c r="T10" s="9">
@@ -1228,12 +1228,12 @@
         <v>0</v>
       </c>
       <c r="V10" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1243,7 +1243,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7">
         <f>SUM(C4:C10)</f>
-        <v>14433884</v>
+        <v>11254604</v>
       </c>
       <c r="D11" s="7">
         <f>SUM(D4:D10)</f>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="E11" s="7">
         <f>SUM(E4:E10)</f>
-        <v>14433884</v>
+        <v>11254604</v>
       </c>
       <c r="F11" s="7">
         <f>SUM(F4:F10)</f>
@@ -1263,11 +1263,11 @@
       </c>
       <c r="H11" s="7">
         <f>(E11+B11)/(X11+1)</f>
-        <v>515495.85714285716</v>
+        <v>416837.18518518517</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="4"/>
-        <v>4108501.9814285715</v>
+        <v>3363876.0844444446</v>
       </c>
       <c r="J11" s="7">
         <f>B11*O11</f>
@@ -1280,21 +1280,21 @@
       </c>
       <c r="M11" s="7">
         <f t="shared" si="7"/>
-        <v>51652.891497280274</v>
+        <v>47529.895688162505</v>
       </c>
       <c r="N11" s="6">
-        <v>7.97</v>
+        <v>8.07</v>
       </c>
       <c r="O11" s="6"/>
       <c r="P11" s="6">
-        <v>9.98</v>
+        <v>8.77</v>
       </c>
       <c r="Q11" s="6" t="e">
         <f>AVERAGE(Q4:Q10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="12">
-        <v>0.67</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="S11" s="12"/>
       <c r="T11" s="7">
@@ -1306,12 +1306,12 @@
         <v>0</v>
       </c>
       <c r="V11" s="6">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W11" s="6"/>
       <c r="X11" s="6">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1319,13 +1319,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="9">
-        <v>3336041</v>
+      <c r="C12" s="2">
+        <v>3049596</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9">
         <f t="shared" si="0"/>
-        <v>3336041</v>
+        <v>3049596</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="1"/>
@@ -1337,11 +1337,11 @@
       </c>
       <c r="H12" s="9">
         <f t="shared" si="3"/>
-        <v>119144.32142857143</v>
+        <v>112948</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="4"/>
-        <v>427728.11392857146</v>
+        <v>466475.24</v>
       </c>
       <c r="J12" s="9">
         <f t="shared" si="5"/>
@@ -1354,18 +1354,18 @@
       </c>
       <c r="M12" s="9">
         <f t="shared" si="7"/>
-        <v>13238.257936507936</v>
+        <v>11294.8</v>
       </c>
       <c r="N12" s="8">
-        <v>3.59</v>
+        <v>4.13</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="11">
-        <v>0.78</v>
+        <v>0.73</v>
       </c>
       <c r="S12" s="11"/>
       <c r="T12" s="9">
@@ -1377,12 +1377,12 @@
         <v>0</v>
       </c>
       <c r="V12" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1391,12 +1391,12 @@
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9">
-        <v>959072</v>
+        <v>241401</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9">
         <f t="shared" ref="E13" si="11">C13-D13</f>
-        <v>959072</v>
+        <v>241401</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" ref="F13" si="12">C13*W13/V13</f>
@@ -1408,11 +1408,11 @@
       </c>
       <c r="H13" s="9">
         <f t="shared" ref="H13" si="14">(E13+B13)/(X13+1)</f>
-        <v>34252.571428571428</v>
+        <v>8940.7777777777774</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" ref="I13" si="15">H13*N13</f>
-        <v>233602.53714285715</v>
+        <v>62048.997777777775</v>
       </c>
       <c r="J13" s="9">
         <f t="shared" ref="J13" si="16">B13*O13</f>
@@ -1425,18 +1425,18 @@
       </c>
       <c r="M13" s="9">
         <f t="shared" ref="M13" si="18">H13/P13</f>
-        <v>3425.2571428571428</v>
+        <v>1117.5972222222222</v>
       </c>
       <c r="N13" s="20">
-        <v>6.82</v>
+        <v>6.94</v>
       </c>
       <c r="O13" s="18"/>
       <c r="P13" s="18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q13" s="18"/>
       <c r="R13" s="19">
-        <v>0.61799999999999999</v>
+        <v>0.65</v>
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="9">
@@ -1448,12 +1448,12 @@
         <v>0</v>
       </c>
       <c r="V13" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" ref="X13" si="21">V13-W13</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1462,10 +1462,9 @@
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-      <c r="I15" s="2"/>
-      <c r="M15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -1497,7 +1496,7 @@
     <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <f>C11</f>
-        <v>14433884</v>
+        <v>11254604</v>
       </c>
       <c r="B18" s="13">
         <f>D11</f>
@@ -1517,7 +1516,7 @@
       </c>
       <c r="F18" s="13">
         <f>$C$11-E18</f>
-        <v>14433884</v>
+        <v>11254604</v>
       </c>
       <c r="M18" s="1"/>
     </row>
@@ -1532,15 +1531,15 @@
       </c>
       <c r="D19" s="13">
         <f t="shared" ref="D19:D23" si="22">C19*$X$11</f>
-        <v>945000</v>
+        <v>910000</v>
       </c>
       <c r="E19" s="13">
         <f t="shared" ref="E19:E23" si="23">$D$11+D19</f>
-        <v>945000</v>
+        <v>910000</v>
       </c>
       <c r="F19" s="13">
         <f t="shared" ref="F19:F23" si="24">$C$11-E19</f>
-        <v>13488884</v>
+        <v>10344604</v>
       </c>
       <c r="M19" s="1"/>
     </row>
@@ -1555,15 +1554,15 @@
       </c>
       <c r="D20" s="13">
         <f t="shared" si="22"/>
-        <v>1890000</v>
+        <v>1820000</v>
       </c>
       <c r="E20" s="13">
         <f t="shared" si="23"/>
-        <v>1890000</v>
+        <v>1820000</v>
       </c>
       <c r="F20" s="13">
         <f t="shared" si="24"/>
-        <v>12543884</v>
+        <v>9434604</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1577,15 +1576,15 @@
       </c>
       <c r="D21" s="13">
         <f t="shared" si="22"/>
-        <v>2835000</v>
+        <v>2730000</v>
       </c>
       <c r="E21" s="13">
         <f t="shared" si="23"/>
-        <v>2835000</v>
+        <v>2730000</v>
       </c>
       <c r="F21" s="13">
         <f t="shared" si="24"/>
-        <v>11598884</v>
+        <v>8524604</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1599,15 +1598,15 @@
       </c>
       <c r="D22" s="13">
         <f t="shared" si="22"/>
-        <v>3780000</v>
+        <v>3640000</v>
       </c>
       <c r="E22" s="13">
         <f t="shared" si="23"/>
-        <v>3780000</v>
+        <v>3640000</v>
       </c>
       <c r="F22" s="13">
         <f t="shared" si="24"/>
-        <v>10653884</v>
+        <v>7614604</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1621,15 +1620,15 @@
       </c>
       <c r="D23" s="13">
         <f t="shared" si="22"/>
-        <v>4725000</v>
+        <v>4550000</v>
       </c>
       <c r="E23" s="13">
         <f t="shared" si="23"/>
-        <v>4725000</v>
+        <v>4550000</v>
       </c>
       <c r="F23" s="13">
         <f t="shared" si="24"/>
-        <v>9708884</v>
+        <v>6704604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: reorganize excel files into archive structure for 2025
Move daily excel files from root folders into corresponding year/month archive structure
Delete old files from root folders after archiving
Update template.xlsx file
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Work\1. Daily\Production follow up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6DAA9B-1861-495D-A999-32CC1AD127F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80303076-07AF-4004-915A-382F5F527284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -335,6 +335,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,6 +641,7 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.42578125" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
   </cols>
@@ -653,7 +657,7 @@
       </c>
       <c r="B2" s="4">
         <f ca="1">TODAY() - 1</f>
-        <v>46022</v>
+        <v>46024</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -736,12 +740,12 @@
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9">
-        <v>2724653</v>
+        <v>2934984</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9">
         <f>C4-D4</f>
-        <v>2724653</v>
+        <v>2934984</v>
       </c>
       <c r="F4" s="9">
         <f>C4*W4/V4</f>
@@ -753,11 +757,11 @@
       </c>
       <c r="H4" s="9">
         <f>(E4+B4)/(X4+1)</f>
-        <v>97309.03571428571</v>
+        <v>108703.11111111111</v>
       </c>
       <c r="I4" s="9">
         <f>H4*N4</f>
-        <v>686028.70178571425</v>
+        <v>682655.53777777776</v>
       </c>
       <c r="J4" s="9">
         <f>B4*O4</f>
@@ -770,10 +774,10 @@
       </c>
       <c r="M4" s="9">
         <f>H4/P4</f>
-        <v>9730.903571428571</v>
+        <v>10870.31111111111</v>
       </c>
       <c r="N4" s="8">
-        <v>7.05</v>
+        <v>6.28</v>
       </c>
       <c r="O4" s="8"/>
       <c r="P4" s="8">
@@ -781,7 +785,7 @@
       </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="11">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="S4" s="11"/>
       <c r="T4" s="9">
@@ -793,12 +797,12 @@
         <v>0</v>
       </c>
       <c r="V4" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W4" s="8"/>
       <c r="X4" s="8">
         <f>V4-W4</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -807,12 +811,12 @@
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9">
-        <v>1530868</v>
+        <v>1496352</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9">
         <f t="shared" ref="E5:E9" si="0">C5-D5</f>
-        <v>1530868</v>
+        <v>1496352</v>
       </c>
       <c r="F5" s="9">
         <f t="shared" ref="F5:F9" si="1">C5*W5/V5</f>
@@ -824,11 +828,11 @@
       </c>
       <c r="H5" s="9">
         <f t="shared" ref="H5:H9" si="3">(E5+B5)/(X5+1)</f>
-        <v>54673.857142857145</v>
+        <v>55420.444444444445</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" ref="I5:I9" si="4">H5*N5</f>
-        <v>370688.75142857147</v>
+        <v>371871.18222222221</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" ref="J5:J9" si="5">B5*O5</f>
@@ -841,18 +845,18 @@
       </c>
       <c r="M5" s="9">
         <f t="shared" ref="M5:M9" si="7">H5/P5</f>
-        <v>4970.3506493506493</v>
+        <v>5542.0444444444447</v>
       </c>
       <c r="N5" s="8">
-        <v>6.78</v>
+        <v>6.71</v>
       </c>
       <c r="O5" s="8"/>
       <c r="P5" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="11">
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="S5" s="11"/>
       <c r="T5" s="9">
@@ -864,12 +868,12 @@
         <v>0</v>
       </c>
       <c r="V5" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W5" s="8"/>
       <c r="X5" s="8">
         <f t="shared" ref="X5:X12" si="10">V5-W5</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -878,12 +882,12 @@
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9">
-        <v>2684219</v>
+        <v>2665075</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9">
         <f t="shared" si="0"/>
-        <v>2684219</v>
+        <v>2665075</v>
       </c>
       <c r="F6" s="9">
         <f t="shared" si="1"/>
@@ -895,11 +899,11 @@
       </c>
       <c r="H6" s="9">
         <f t="shared" si="3"/>
-        <v>95864.96428571429</v>
+        <v>98706.481481481474</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" si="4"/>
-        <v>806224.34964285721</v>
+        <v>718583.18518518517</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" si="5"/>
@@ -912,10 +916,10 @@
       </c>
       <c r="M6" s="9">
         <f t="shared" si="7"/>
-        <v>9586.4964285714286</v>
+        <v>9870.6481481481478</v>
       </c>
       <c r="N6" s="8">
-        <v>8.41</v>
+        <v>7.28</v>
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8">
@@ -923,7 +927,7 @@
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="11">
-        <v>0.63</v>
+        <v>0.62149999999999994</v>
       </c>
       <c r="S6" s="11"/>
       <c r="T6" s="9">
@@ -935,12 +939,12 @@
         <v>0</v>
       </c>
       <c r="V6" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -949,12 +953,12 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9">
-        <v>2343006</v>
+        <v>2104429</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9">
         <f t="shared" si="0"/>
-        <v>2343006</v>
+        <v>2104429</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" si="1"/>
@@ -966,11 +970,11 @@
       </c>
       <c r="H7" s="9">
         <f t="shared" si="3"/>
-        <v>83678.78571428571</v>
+        <v>77941.814814814818</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" si="4"/>
-        <v>617549.43857142853</v>
+        <v>631328.69999999995</v>
       </c>
       <c r="J7" s="9">
         <f t="shared" si="5"/>
@@ -983,10 +987,10 @@
       </c>
       <c r="M7" s="9">
         <f t="shared" si="7"/>
-        <v>8367.8785714285714</v>
+        <v>7794.1814814814816</v>
       </c>
       <c r="N7" s="8">
-        <v>7.38</v>
+        <v>8.1</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8">
@@ -994,7 +998,7 @@
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="11">
-        <v>0.71</v>
+        <v>0.6925</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="9">
@@ -1006,12 +1010,12 @@
         <v>0</v>
       </c>
       <c r="V7" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1020,12 +1024,12 @@
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9">
-        <v>3107863</v>
+        <v>2701433</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9">
         <f t="shared" si="0"/>
-        <v>3107863</v>
+        <v>2701433</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="1"/>
@@ -1037,11 +1041,11 @@
       </c>
       <c r="H8" s="9">
         <f t="shared" si="3"/>
-        <v>110995.10714285714</v>
+        <v>100053.07407407407</v>
       </c>
       <c r="I8" s="9">
         <f t="shared" si="4"/>
-        <v>724798.04964285716</v>
+        <v>707375.23370370374</v>
       </c>
       <c r="J8" s="9">
         <f t="shared" si="5"/>
@@ -1054,10 +1058,10 @@
       </c>
       <c r="M8" s="9">
         <f t="shared" si="7"/>
-        <v>11099.510714285714</v>
+        <v>10005.307407407407</v>
       </c>
       <c r="N8" s="8">
-        <v>6.53</v>
+        <v>7.07</v>
       </c>
       <c r="O8" s="8"/>
       <c r="P8" s="8">
@@ -1065,7 +1069,7 @@
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="11">
-        <v>0.68</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="S8" s="11"/>
       <c r="T8" s="9">
@@ -1077,12 +1081,12 @@
         <v>0</v>
       </c>
       <c r="V8" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1091,12 +1095,12 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9">
-        <v>4032281</v>
+        <v>3615050</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9">
         <f t="shared" si="0"/>
-        <v>4032281</v>
+        <v>3615050</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="1"/>
@@ -1108,11 +1112,11 @@
       </c>
       <c r="H9" s="9">
         <f t="shared" si="3"/>
-        <v>144010.03571428571</v>
+        <v>133890.74074074073</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="4"/>
-        <v>1137679.2821428571</v>
+        <v>1026941.9814814813</v>
       </c>
       <c r="J9" s="9">
         <f t="shared" si="5"/>
@@ -1125,10 +1129,10 @@
       </c>
       <c r="M9" s="9">
         <f t="shared" si="7"/>
-        <v>14401.003571428571</v>
+        <v>13389.074074074073</v>
       </c>
       <c r="N9" s="8">
-        <v>7.9</v>
+        <v>7.67</v>
       </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8">
@@ -1148,12 +1152,12 @@
         <v>0</v>
       </c>
       <c r="V9" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1162,12 +1166,12 @@
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9">
-        <v>3336726</v>
+        <v>3140225</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9">
         <f>C10-D10</f>
-        <v>3336726</v>
+        <v>3140225</v>
       </c>
       <c r="F10" s="9">
         <f>C10*W10/V10</f>
@@ -1179,11 +1183,11 @@
       </c>
       <c r="H10" s="9">
         <f>(E10+B10)/(X10+1)</f>
-        <v>119168.78571428571</v>
+        <v>116304.62962962964</v>
       </c>
       <c r="I10" s="9">
         <f>H10*N10</f>
-        <v>499317.2121428572</v>
+        <v>482664.21296296304</v>
       </c>
       <c r="J10" s="9">
         <f>B10*O10</f>
@@ -1196,18 +1200,18 @@
       </c>
       <c r="M10" s="9">
         <f>H10/P10</f>
-        <v>11822.300170068027</v>
+        <v>11630.462962962964</v>
       </c>
       <c r="N10" s="8">
-        <v>4.1900000000000004</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8">
-        <v>10.08</v>
+        <v>10</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="11">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="S10" s="11"/>
       <c r="T10" s="9">
@@ -1219,12 +1223,12 @@
         <v>0</v>
       </c>
       <c r="V10" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f>V10-W10</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1284,12 +1288,12 @@
         <v>0</v>
       </c>
       <c r="V11" s="8">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W11" s="8"/>
       <c r="X11" s="8">
         <f>V11-W11</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1297,43 +1301,43 @@
         <v>42</v>
       </c>
       <c r="B12" s="7">
-        <f>SUM(B4:B9)</f>
+        <f>SUM(B4:B11)</f>
         <v>0</v>
       </c>
       <c r="C12" s="7">
-        <f>SUM(C4:C9)</f>
-        <v>16422890</v>
+        <f>SUM(C4:C11)</f>
+        <v>18657548</v>
       </c>
       <c r="D12" s="7">
-        <f>SUM(D4:D9)</f>
+        <f t="shared" ref="D12:G12" si="11">SUM(D4:D11)</f>
         <v>0</v>
       </c>
       <c r="E12" s="7">
-        <f>SUM(E4:E9)</f>
-        <v>16422890</v>
+        <f t="shared" si="11"/>
+        <v>18657548</v>
       </c>
       <c r="F12" s="7">
-        <f>SUM(F4:F9)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G12" s="7">
-        <f>SUM(G4:G9)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H12" s="7">
         <f>(E12+B12)/(X12+1)</f>
-        <v>586531.78571428568</v>
+        <v>691020.29629629629</v>
       </c>
       <c r="I12" s="7">
         <f>H12*N12</f>
-        <v>4328604.5785714285</v>
+        <v>4665374.171851851</v>
       </c>
       <c r="J12" s="7" t="e">
         <f>B12*O12</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K12" s="7">
-        <f>SUM(K4:K9)</f>
+        <f>SUM(K4:K11)</f>
         <v>0</v>
       </c>
       <c r="L12" s="12" t="e">
@@ -1342,10 +1346,10 @@
       </c>
       <c r="M12" s="7">
         <f>H12/P12</f>
-        <v>58653.178571428565</v>
-      </c>
-      <c r="N12" s="6">
-        <v>7.38</v>
+        <v>69102.029629629629</v>
+      </c>
+      <c r="N12" s="22">
+        <v>6.7514285714285709</v>
       </c>
       <c r="O12" s="6" t="e">
         <f>AVERAGE(O4:O9)</f>
@@ -1359,7 +1363,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="12">
-        <v>0.68630000000000002</v>
+        <v>0.61124999999999985</v>
       </c>
       <c r="S12" s="12" t="e">
         <f>AVERAGE(S4:S9)</f>
@@ -1374,12 +1378,12 @@
         <v>0</v>
       </c>
       <c r="V12" s="6">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W12" s="6"/>
       <c r="X12" s="6">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1423,7 +1427,7 @@
     <row r="18" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <f>C12</f>
-        <v>16422890</v>
+        <v>18657548</v>
       </c>
       <c r="B18" s="13">
         <f>D12</f>
@@ -1434,16 +1438,16 @@
         <v>0</v>
       </c>
       <c r="D18" s="13">
-        <f>C18*$X$12</f>
+        <f t="shared" ref="D18:D23" si="12">C18*$X$12</f>
         <v>0</v>
       </c>
       <c r="E18" s="13">
-        <f>$D$12+D18</f>
+        <f t="shared" ref="E18:E23" si="13">$D$12+D18</f>
         <v>0</v>
       </c>
       <c r="F18" s="13">
-        <f>$C$12-E18</f>
-        <v>16422890</v>
+        <f t="shared" ref="F18:F23" si="14">$C$12-E18</f>
+        <v>18657548</v>
       </c>
       <c r="M18" s="1"/>
     </row>
@@ -1457,16 +1461,16 @@
         <v>35000</v>
       </c>
       <c r="D19" s="13">
-        <f>C19*$X$12</f>
-        <v>945000</v>
+        <f t="shared" si="12"/>
+        <v>910000</v>
       </c>
       <c r="E19" s="13">
-        <f>$D$12+D19</f>
-        <v>945000</v>
+        <f t="shared" si="13"/>
+        <v>910000</v>
       </c>
       <c r="F19" s="13">
-        <f>$C$12-E19</f>
-        <v>15477890</v>
+        <f t="shared" si="14"/>
+        <v>17747548</v>
       </c>
       <c r="M19" s="1"/>
     </row>
@@ -1476,20 +1480,20 @@
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="13">
-        <f t="shared" ref="C20:C23" si="11">C19+35000</f>
+        <f t="shared" ref="C20:C23" si="15">C19+35000</f>
         <v>70000</v>
       </c>
       <c r="D20" s="13">
-        <f>C20*$X$12</f>
-        <v>1890000</v>
+        <f t="shared" si="12"/>
+        <v>1820000</v>
       </c>
       <c r="E20" s="13">
-        <f>$D$12+D20</f>
-        <v>1890000</v>
+        <f t="shared" si="13"/>
+        <v>1820000</v>
       </c>
       <c r="F20" s="13">
-        <f>$C$12-E20</f>
-        <v>14532890</v>
+        <f t="shared" si="14"/>
+        <v>16837548</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1498,20 +1502,20 @@
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>105000</v>
       </c>
       <c r="D21" s="13">
-        <f>C21*$X$12</f>
-        <v>2835000</v>
+        <f t="shared" si="12"/>
+        <v>2730000</v>
       </c>
       <c r="E21" s="13">
-        <f>$D$12+D21</f>
-        <v>2835000</v>
+        <f t="shared" si="13"/>
+        <v>2730000</v>
       </c>
       <c r="F21" s="13">
-        <f>$C$12-E21</f>
-        <v>13587890</v>
+        <f t="shared" si="14"/>
+        <v>15927548</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1520,20 +1524,20 @@
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>140000</v>
       </c>
       <c r="D22" s="13">
-        <f>C22*$X$12</f>
-        <v>3780000</v>
+        <f t="shared" si="12"/>
+        <v>3640000</v>
       </c>
       <c r="E22" s="13">
-        <f>$D$12+D22</f>
-        <v>3780000</v>
+        <f t="shared" si="13"/>
+        <v>3640000</v>
       </c>
       <c r="F22" s="13">
-        <f>$C$12-E22</f>
-        <v>12642890</v>
+        <f t="shared" si="14"/>
+        <v>15017548</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1542,20 +1546,20 @@
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>175000</v>
       </c>
       <c r="D23" s="13">
-        <f>C23*$X$12</f>
-        <v>4725000</v>
+        <f t="shared" si="12"/>
+        <v>4550000</v>
       </c>
       <c r="E23" s="13">
-        <f>$D$12+D23</f>
-        <v>4725000</v>
+        <f t="shared" si="13"/>
+        <v>4550000</v>
       </c>
       <c r="F23" s="13">
-        <f>$C$12-E23</f>
-        <v>11697890</v>
+        <f t="shared" si="14"/>
+        <v>14107548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>